<commit_message>
Actualizacion plan de metricas
</commit_message>
<xml_diff>
--- a/Organización/Métricas y monitoreo/Plan_Métricas_aaaa.xlsx
+++ b/Organización/Métricas y monitoreo/Plan_Métricas_aaaa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-1365" yWindow="300" windowWidth="16605" windowHeight="9435" tabRatio="971" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="-1365" yWindow="300" windowWidth="16605" windowHeight="9435" tabRatio="971" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Objetivos de Medición" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,9 @@
     <sheet name="Apego a Auditorias Funcionales" sheetId="19" r:id="rId7"/>
     <sheet name="Índice de Satisfacción" sheetId="20" r:id="rId8"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="125">
   <si>
     <t>Objetivos/Necesidades de Negocio y  Medición</t>
   </si>
@@ -145,9 +148,6 @@
     <t>Desviacion del costo</t>
   </si>
   <si>
-    <t>Auditor</t>
-  </si>
-  <si>
     <t>Conocer cual es el apego y consistencia en la generación y uso de las herramientas de trabajo</t>
   </si>
   <si>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>Dirección</t>
-  </si>
-  <si>
-    <t>Soporte TI</t>
   </si>
   <si>
     <t xml:space="preserve">Conocer si los servicios ofrecidos al cliente cumplen con sus espectativas. </t>
@@ -367,15 +364,6 @@
     </r>
   </si>
   <si>
-    <t>Si la desviacion es de 0% a 30%</t>
-  </si>
-  <si>
-    <t>Si la desvacion es mayor al 30% y menor o igual a 65%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si la desviación es menor que 0 o Si la desviacion es mayor a 65% </t>
-  </si>
-  <si>
     <t xml:space="preserve">Que el índice de satisfacción sea mayor o igual a 85% </t>
   </si>
   <si>
@@ -416,6 +404,30 @@
   </si>
   <si>
     <t>Ingresar al check list de calidad correspondiente. Tomar el valor ubicado en la pestaña "Resumen" -&gt; seccion Funcionales. Registrar los valores acorde a su orden en el archivo concentrado de metricas pestaña "Funcional"</t>
+  </si>
+  <si>
+    <t>Si la desviacion es de 0% a 10%</t>
+  </si>
+  <si>
+    <t>Si la desvacion es mayor al 10% y menor o igual a 30%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si la desviación es menor que 0 o Si la desviacion es mayor a 30% </t>
+  </si>
+  <si>
+    <t>Jovanny Zepeda</t>
+  </si>
+  <si>
+    <t>Ingresar a bitrix (ruta de ubicación) tomar las horas registradas para cada sección del ciclo de vida, multiplicarla por el costo en horas dependiendo del puesto (se encuentra ubicada en estimación de proyecto pestaña costo por hora personal), finalmente hacer la sumatoria de los costos por horas de cada etapa y registrarlos en la pestaña desviación costos del concentrado de metricas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingresar a Bitrix() ,tomar las horas registradas para cada sección del ciclo de vida , registrar el acomulado total en el documento concentrado de metricas pestaña desviación de esfuerzo. </t>
+  </si>
+  <si>
+    <t>Crear plan de acción para aumentar el promedio de satisfacción.</t>
+  </si>
+  <si>
+    <t>calidad</t>
   </si>
 </sst>
 </file>
@@ -969,6 +981,15 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -983,15 +1004,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="60">
@@ -1392,11 +1404,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="80939648"/>
-        <c:axId val="80949632"/>
+        <c:axId val="84988672"/>
+        <c:axId val="84990208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80939648"/>
+        <c:axId val="84988672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,7 +1418,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80949632"/>
+        <c:crossAx val="84990208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1414,7 +1426,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80949632"/>
+        <c:axId val="84990208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1428,7 +1440,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80939648"/>
+        <c:crossAx val="84988672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1764,11 +1776,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="81039744"/>
-        <c:axId val="81041280"/>
+        <c:axId val="39489920"/>
+        <c:axId val="39491456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81039744"/>
+        <c:axId val="39489920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1778,7 +1790,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81041280"/>
+        <c:crossAx val="39491456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1786,7 +1798,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81041280"/>
+        <c:axId val="39491456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1800,7 +1812,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81039744"/>
+        <c:crossAx val="39489920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1824,6 +1836,469 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-MX"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX"/>
+              <a:t>Costo</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]Desviacion de costos'!$C$18:$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Planeado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'[1]Desviacion de costos'!$B$20:$B$27</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Prospectación</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ventas</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Planeación</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Compras</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Implementación</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Cierre</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Garantia</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Soporte</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[1]Desviacion de costos'!$C$20:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-15F3-4939-9302-9660B3AF6930}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]Desviacion de costos'!$D$18:$D$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'[1]Desviacion de costos'!$B$20:$B$27</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Prospectación</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ventas</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Planeación</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Compras</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Implementación</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Cierre</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Garantia</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Soporte</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[1]Desviacion de costos'!$D$20:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-15F3-4939-9302-9660B3AF6930}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="110881792"/>
+        <c:axId val="187134720"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="110881792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="187134720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="187134720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="110881792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-MX"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Desviación</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]Desviacion de costos'!$E$18:$E$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Desviación</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'[1]Desviacion de costos'!$B$20:$B$27</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Prospectación</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ventas</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Planeación</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Compras</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Implementación</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Cierre</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Garantia</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Soporte</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[1]Desviacion de costos'!$E$20:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4C53-4413-9153-0DEA66086AD7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="111411584"/>
+        <c:axId val="111413120"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="111411584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="111413120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="111413120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="111411584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-MX"/>
@@ -2132,11 +2607,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="86783872"/>
-        <c:axId val="86785408"/>
+        <c:axId val="39577472"/>
+        <c:axId val="39579008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86783872"/>
+        <c:axId val="39577472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2146,7 +2621,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86785408"/>
+        <c:crossAx val="39579008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2154,7 +2629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86785408"/>
+        <c:axId val="39579008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2168,7 +2643,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86783872"/>
+        <c:crossAx val="39577472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2191,7 +2666,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-MX"/>
@@ -2500,11 +2975,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="87104512"/>
-        <c:axId val="87147264"/>
+        <c:axId val="39619584"/>
+        <c:axId val="39625472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87104512"/>
+        <c:axId val="39619584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2514,7 +2989,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87147264"/>
+        <c:crossAx val="39625472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2522,7 +2997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87147264"/>
+        <c:axId val="39625472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2536,7 +3011,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87104512"/>
+        <c:crossAx val="39619584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2559,7 +3034,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-MX"/>
@@ -2868,11 +3343,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="86876160"/>
-        <c:axId val="86877696"/>
+        <c:axId val="39678336"/>
+        <c:axId val="39679872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86876160"/>
+        <c:axId val="39678336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2882,7 +3357,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86877696"/>
+        <c:crossAx val="39679872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2890,7 +3365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86877696"/>
+        <c:axId val="39679872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2904,7 +3379,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86876160"/>
+        <c:crossAx val="39678336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2927,7 +3402,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-MX"/>
@@ -3236,11 +3711,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="87014400"/>
-        <c:axId val="87020288"/>
+        <c:axId val="39712256"/>
+        <c:axId val="39713792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87014400"/>
+        <c:axId val="39712256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3250,7 +3725,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87020288"/>
+        <c:crossAx val="39713792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3258,7 +3733,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87020288"/>
+        <c:axId val="39713792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3272,7 +3747,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87014400"/>
+        <c:crossAx val="39712256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3357,6 +3832,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1409700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2400300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="3 Gráfico">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1609725</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>5553075</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="4 Gráfico">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3511,6 +4062,276 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Desviacion de esfuerzo"/>
+      <sheetName val="Desviacion de costos"/>
+      <sheetName val="Apego a Procesos"/>
+      <sheetName val="Apego a Productos"/>
+      <sheetName val="Física"/>
+      <sheetName val="Funcional"/>
+      <sheetName val="Indice de Satisfacción"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="19">
+          <cell r="D19" t="str">
+            <v xml:space="preserve">Real </v>
+          </cell>
+          <cell r="E19" t="str">
+            <v>Desviación</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20" t="str">
+            <v>Prospectación</v>
+          </cell>
+          <cell r="C20">
+            <v>0</v>
+          </cell>
+          <cell r="D20">
+            <v>0</v>
+          </cell>
+          <cell r="E20" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21" t="str">
+            <v>Ventas</v>
+          </cell>
+          <cell r="C21">
+            <v>0</v>
+          </cell>
+          <cell r="D21">
+            <v>0</v>
+          </cell>
+          <cell r="E21" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22" t="str">
+            <v>Planeación</v>
+          </cell>
+          <cell r="C22">
+            <v>0</v>
+          </cell>
+          <cell r="D22">
+            <v>0</v>
+          </cell>
+          <cell r="E22" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23" t="str">
+            <v>Compras</v>
+          </cell>
+          <cell r="C23">
+            <v>0</v>
+          </cell>
+          <cell r="D23">
+            <v>0</v>
+          </cell>
+          <cell r="E23" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24" t="str">
+            <v>Implementación</v>
+          </cell>
+          <cell r="C24">
+            <v>0</v>
+          </cell>
+          <cell r="D24">
+            <v>0</v>
+          </cell>
+          <cell r="E24" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25" t="str">
+            <v>Cierre</v>
+          </cell>
+          <cell r="C25">
+            <v>0</v>
+          </cell>
+          <cell r="D25">
+            <v>0</v>
+          </cell>
+          <cell r="E25" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26" t="str">
+            <v>Garantia</v>
+          </cell>
+          <cell r="C26">
+            <v>0</v>
+          </cell>
+          <cell r="D26">
+            <v>0</v>
+          </cell>
+          <cell r="E26" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27" t="str">
+            <v>Soporte</v>
+          </cell>
+          <cell r="C27">
+            <v>0</v>
+          </cell>
+          <cell r="D27">
+            <v>0</v>
+          </cell>
+          <cell r="E27" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="19">
+          <cell r="C19" t="str">
+            <v>Planeado</v>
+          </cell>
+          <cell r="D19" t="str">
+            <v xml:space="preserve">Real </v>
+          </cell>
+          <cell r="E19" t="str">
+            <v>Desviación</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20" t="str">
+            <v>Prospectación</v>
+          </cell>
+          <cell r="C20">
+            <v>0</v>
+          </cell>
+          <cell r="D20">
+            <v>0</v>
+          </cell>
+          <cell r="E20" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21" t="str">
+            <v>Ventas</v>
+          </cell>
+          <cell r="C21">
+            <v>0</v>
+          </cell>
+          <cell r="D21">
+            <v>0</v>
+          </cell>
+          <cell r="E21" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22" t="str">
+            <v>Planeación</v>
+          </cell>
+          <cell r="C22">
+            <v>0</v>
+          </cell>
+          <cell r="D22">
+            <v>0</v>
+          </cell>
+          <cell r="E22" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23" t="str">
+            <v>Compras</v>
+          </cell>
+          <cell r="C23">
+            <v>0</v>
+          </cell>
+          <cell r="D23">
+            <v>0</v>
+          </cell>
+          <cell r="E23" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24" t="str">
+            <v>Implementación</v>
+          </cell>
+          <cell r="C24">
+            <v>0</v>
+          </cell>
+          <cell r="D24">
+            <v>0</v>
+          </cell>
+          <cell r="E24" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25" t="str">
+            <v>Cierre</v>
+          </cell>
+          <cell r="C25">
+            <v>0</v>
+          </cell>
+          <cell r="D25">
+            <v>0</v>
+          </cell>
+          <cell r="E25" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26" t="str">
+            <v>Garantia</v>
+          </cell>
+          <cell r="C26">
+            <v>0</v>
+          </cell>
+          <cell r="D26">
+            <v>0</v>
+          </cell>
+          <cell r="E26" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27" t="str">
+            <v>Soporte</v>
+          </cell>
+          <cell r="C27">
+            <v>0</v>
+          </cell>
+          <cell r="D27">
+            <v>0</v>
+          </cell>
+          <cell r="E27" t="e">
+            <v>#DIV/0!</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3806,7 +4627,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3839,21 +4660,21 @@
     </row>
     <row r="3" spans="1:7" ht="24.6" customHeight="1">
       <c r="B3" s="63" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="11" customFormat="1" ht="21" customHeight="1">
       <c r="B4" s="63"/>
       <c r="C4" s="23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="B5" s="63" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>22</v>
@@ -3864,30 +4685,30 @@
       <c r="A6" s="22"/>
       <c r="B6" s="63"/>
       <c r="C6" s="23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:7">
       <c r="B7" s="63"/>
       <c r="C7" s="23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:7">
       <c r="B8" s="63"/>
       <c r="C8" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D8" s="22"/>
     </row>
     <row r="9" spans="1:7" ht="30">
       <c r="B9" s="24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3923,25 +4744,29 @@
     <row r="13" spans="1:7" s="5" customFormat="1">
       <c r="A13" s="3"/>
       <c r="B13" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="56" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="56"/>
       <c r="E13" s="57" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F13" s="58"/>
     </row>
     <row r="14" spans="1:7" s="5" customFormat="1" ht="19.149999999999999" customHeight="1">
       <c r="A14" s="3"/>
-      <c r="B14" s="20"/>
+      <c r="B14" s="20" t="s">
+        <v>33</v>
+      </c>
       <c r="C14" s="54" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D14" s="55"/>
-      <c r="E14" s="57"/>
+      <c r="E14" s="57" t="s">
+        <v>120</v>
+      </c>
       <c r="F14" s="58"/>
     </row>
     <row r="15" spans="1:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1">
@@ -4005,15 +4830,15 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="89.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="109.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="27" width="11.42578125" style="1"/>
@@ -4035,15 +4860,15 @@
         <v>3</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="2:3" outlineLevel="1">
       <c r="B3" s="26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
@@ -4075,7 +4900,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="70" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
@@ -4086,10 +4911,10 @@
     </row>
     <row r="10" spans="2:3" outlineLevel="1">
       <c r="B10" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="31" t="s">
         <v>94</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="11" spans="2:3" outlineLevel="1">
@@ -4099,7 +4924,9 @@
       <c r="C11" s="67"/>
     </row>
     <row r="12" spans="2:3" ht="33.75" customHeight="1" outlineLevel="1">
-      <c r="B12" s="66"/>
+      <c r="B12" s="66" t="s">
+        <v>122</v>
+      </c>
       <c r="C12" s="66"/>
     </row>
     <row r="13" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
@@ -4113,7 +4940,7 @@
     <row r="14" spans="2:3" outlineLevel="1">
       <c r="B14" s="30"/>
       <c r="C14" s="30" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:3" outlineLevel="1">
@@ -4138,52 +4965,52 @@
     </row>
     <row r="18" spans="2:3" outlineLevel="1">
       <c r="B18" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
       <c r="B19" s="30"/>
       <c r="C19" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
       <c r="B20" s="67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C20" s="67"/>
     </row>
     <row r="21" spans="2:3" s="18" customFormat="1" outlineLevel="1">
       <c r="B21" s="65" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C21" s="65"/>
     </row>
     <row r="22" spans="2:3" outlineLevel="1">
       <c r="B22" s="33" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="30">
       <c r="B23" s="34" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="30">
       <c r="B24" s="35" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -4364,8 +5191,8 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4394,7 +5221,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="2:3" outlineLevel="1">
@@ -4402,7 +5229,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
@@ -4434,7 +5261,7 @@
         <v>36</v>
       </c>
       <c r="C8" s="70" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
@@ -4445,10 +5272,10 @@
     </row>
     <row r="10" spans="2:3" outlineLevel="1">
       <c r="B10" s="30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="2:3" outlineLevel="1">
@@ -4457,8 +5284,10 @@
       </c>
       <c r="C11" s="67"/>
     </row>
-    <row r="12" spans="2:3" ht="24" customHeight="1" outlineLevel="1">
-      <c r="B12" s="66"/>
+    <row r="12" spans="2:3" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="B12" s="66" t="s">
+        <v>121</v>
+      </c>
       <c r="C12" s="66"/>
     </row>
     <row r="13" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
@@ -4472,7 +5301,7 @@
     <row r="14" spans="2:3" outlineLevel="1">
       <c r="B14" s="30"/>
       <c r="C14" s="30" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:3" outlineLevel="1">
@@ -4497,46 +5326,46 @@
     </row>
     <row r="18" spans="2:3" outlineLevel="1">
       <c r="B18" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
       <c r="B19" s="30"/>
       <c r="C19" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
       <c r="B20" s="67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C20" s="67"/>
     </row>
     <row r="21" spans="2:3" outlineLevel="1">
       <c r="B21" s="33" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="30">
       <c r="B22" s="34" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="30">
       <c r="B23" s="35" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -4717,7 +5546,7 @@
   <dimension ref="B1:AD47"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4749,10 +5578,10 @@
     </row>
     <row r="3" spans="2:3" ht="18" customHeight="1" outlineLevel="1">
       <c r="B3" s="26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
@@ -4781,21 +5610,21 @@
     </row>
     <row r="8" spans="2:3" outlineLevel="1">
       <c r="B8" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="71" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
       <c r="B9" s="30" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C9" s="72"/>
     </row>
     <row r="10" spans="2:3" ht="30" outlineLevel="1">
       <c r="B10" s="30" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C10" s="73"/>
     </row>
@@ -4807,7 +5636,7 @@
     </row>
     <row r="12" spans="2:3" ht="37.5" customHeight="1" outlineLevel="1">
       <c r="B12" s="66" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C12" s="66"/>
     </row>
@@ -4822,7 +5651,7 @@
     <row r="14" spans="2:3" outlineLevel="1">
       <c r="B14" s="30"/>
       <c r="C14" s="30" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:3" outlineLevel="1">
@@ -4842,51 +5671,51 @@
     <row r="17" spans="2:3" outlineLevel="1">
       <c r="B17" s="30"/>
       <c r="C17" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="2:3" outlineLevel="1">
       <c r="B18" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
       <c r="B19" s="30"/>
       <c r="C19" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
       <c r="B20" s="67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C20" s="67"/>
     </row>
     <row r="21" spans="2:3" outlineLevel="1">
       <c r="B21" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="53" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -5067,7 +5896,7 @@
   <dimension ref="B1:AD47"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -5096,15 +5925,15 @@
         <v>3</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="2:3" outlineLevel="1">
       <c r="B3" s="26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
@@ -5133,23 +5962,23 @@
     </row>
     <row r="8" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B8" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="79" t="s">
-        <v>112</v>
+        <v>41</v>
+      </c>
+      <c r="C8" s="74" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
       <c r="B9" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="80"/>
+        <v>105</v>
+      </c>
+      <c r="C9" s="75"/>
     </row>
     <row r="10" spans="2:3" ht="30" outlineLevel="1">
       <c r="B10" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="C10" s="81"/>
+        <v>106</v>
+      </c>
+      <c r="C10" s="76"/>
     </row>
     <row r="11" spans="2:3" outlineLevel="1">
       <c r="B11" s="67" t="s">
@@ -5159,7 +5988,7 @@
     </row>
     <row r="12" spans="2:3" ht="39.75" customHeight="1" outlineLevel="1">
       <c r="B12" s="66" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C12" s="66"/>
     </row>
@@ -5174,7 +6003,7 @@
     <row r="14" spans="2:3" outlineLevel="1">
       <c r="B14" s="30"/>
       <c r="C14" s="30" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:3" outlineLevel="1">
@@ -5194,51 +6023,51 @@
     <row r="17" spans="2:3" outlineLevel="1">
       <c r="B17" s="30"/>
       <c r="C17" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:3" outlineLevel="1">
       <c r="B18" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
       <c r="B19" s="30"/>
       <c r="C19" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
       <c r="B20" s="67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C20" s="67"/>
     </row>
     <row r="21" spans="2:3" outlineLevel="1">
       <c r="B21" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -5419,7 +6248,7 @@
   <dimension ref="B1:AD47"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -5448,15 +6277,15 @@
         <v>3</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="2:3" outlineLevel="1">
       <c r="B3" s="26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
@@ -5485,21 +6314,21 @@
     </row>
     <row r="8" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B8" s="52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="71" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
       <c r="B9" s="52" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C9" s="72"/>
     </row>
     <row r="10" spans="2:3" ht="30" outlineLevel="1">
       <c r="B10" s="52" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C10" s="73"/>
     </row>
@@ -5511,7 +6340,7 @@
     </row>
     <row r="12" spans="2:3" ht="46.9" customHeight="1" outlineLevel="1">
       <c r="B12" s="66" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C12" s="66"/>
     </row>
@@ -5526,7 +6355,7 @@
     <row r="14" spans="2:3" outlineLevel="1">
       <c r="B14" s="30"/>
       <c r="C14" s="30" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:3" outlineLevel="1">
@@ -5546,51 +6375,51 @@
     <row r="17" spans="2:3" outlineLevel="1">
       <c r="B17" s="30"/>
       <c r="C17" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:3" outlineLevel="1">
       <c r="B18" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
       <c r="B19" s="30"/>
       <c r="C19" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
       <c r="B20" s="67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C20" s="67"/>
     </row>
     <row r="21" spans="2:3" outlineLevel="1">
       <c r="B21" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -5771,7 +6600,7 @@
   <dimension ref="B1:AD47"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -5800,7 +6629,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:3" outlineLevel="1">
@@ -5808,7 +6637,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
@@ -5837,21 +6666,21 @@
     </row>
     <row r="8" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B8" s="52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="71" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
       <c r="B9" s="52" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C9" s="72"/>
     </row>
     <row r="10" spans="2:3" ht="30" outlineLevel="1">
       <c r="B10" s="52" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C10" s="73"/>
     </row>
@@ -5863,7 +6692,7 @@
     </row>
     <row r="12" spans="2:3" ht="45.6" customHeight="1" outlineLevel="1">
       <c r="B12" s="66" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C12" s="66"/>
     </row>
@@ -5878,7 +6707,7 @@
     <row r="14" spans="2:3" outlineLevel="1">
       <c r="B14" s="30"/>
       <c r="C14" s="30" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:3" outlineLevel="1">
@@ -5898,51 +6727,51 @@
     <row r="17" spans="2:3" outlineLevel="1">
       <c r="B17" s="30"/>
       <c r="C17" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:3" outlineLevel="1">
       <c r="B18" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
       <c r="B19" s="30"/>
       <c r="C19" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
       <c r="B20" s="67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C20" s="67"/>
     </row>
     <row r="21" spans="2:3" outlineLevel="1">
       <c r="B21" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -6120,8 +6949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6145,7 +6974,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -6153,38 +6982,38 @@
         <v>19</v>
       </c>
       <c r="B3" s="47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="79"/>
+    </row>
+    <row r="5" spans="1:21" ht="184.5" customHeight="1">
+      <c r="A5" s="80"/>
+      <c r="B5" s="80"/>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="78"/>
+      <c r="Q6" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="R6" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="76" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="76"/>
-    </row>
-    <row r="5" spans="1:21" ht="184.5" customHeight="1">
-      <c r="A5" s="77"/>
-      <c r="B5" s="77"/>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="75" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="75"/>
-      <c r="Q6" s="11" t="s">
+      <c r="S6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="T6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="U6" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="T6" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="U6" s="11" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -6192,10 +7021,10 @@
         <v>20</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Q7" s="11">
         <f>AVERAGE(R7:U7)</f>
@@ -6216,13 +7045,13 @@
     </row>
     <row r="8" spans="1:21" ht="30">
       <c r="A8" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="P8" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="P8" s="11" t="s">
-        <v>62</v>
       </c>
       <c r="Q8" s="11">
         <f>AVERAGE(R8:U8)</f>
@@ -6242,16 +7071,16 @@
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="75"/>
+      <c r="B9" s="78"/>
     </row>
     <row r="10" spans="1:21" ht="61.5" customHeight="1">
-      <c r="A10" s="78" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" s="78"/>
+      <c r="A10" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="81"/>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="48" t="s">
@@ -6264,14 +7093,14 @@
     <row r="12" spans="1:21">
       <c r="A12" s="30"/>
       <c r="B12" s="30" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="75" t="s">
+      <c r="A13" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="75"/>
+      <c r="B13" s="78"/>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="48" t="s">
@@ -6284,55 +7113,57 @@
     <row r="15" spans="1:21">
       <c r="A15" s="30"/>
       <c r="B15" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="48" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="30"/>
       <c r="B17" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="75" t="s">
-        <v>104</v>
-      </c>
-      <c r="B18" s="75"/>
+      <c r="A18" s="78" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="78"/>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="74" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="74"/>
+      <c r="A19" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="77"/>
     </row>
     <row r="20" spans="1:2" ht="28.5">
       <c r="A20" s="49" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="28.5">
       <c r="A21" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="B21" s="30"/>
+        <v>104</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="51" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregar diagramas a plan de metricas
</commit_message>
<xml_diff>
--- a/Organización/Métricas y monitoreo/Plan_Métricas_aaaa.xlsx
+++ b/Organización/Métricas y monitoreo/Plan_Métricas_aaaa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-1365" yWindow="300" windowWidth="16605" windowHeight="9435" tabRatio="971" activeTab="1"/>
+    <workbookView xWindow="-1365" yWindow="300" windowWidth="16605" windowHeight="9435" tabRatio="971" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Objetivos de Medición" sheetId="1" r:id="rId1"/>
@@ -1404,11 +1404,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="84988672"/>
-        <c:axId val="84990208"/>
+        <c:axId val="57043200"/>
+        <c:axId val="57044992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="84988672"/>
+        <c:axId val="57043200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1418,7 +1418,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84990208"/>
+        <c:crossAx val="57044992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1426,7 +1426,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84990208"/>
+        <c:axId val="57044992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1440,7 +1440,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84988672"/>
+        <c:crossAx val="57043200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1776,11 +1776,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="39489920"/>
-        <c:axId val="39491456"/>
+        <c:axId val="65261568"/>
+        <c:axId val="65263104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39489920"/>
+        <c:axId val="65261568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1790,7 +1790,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39491456"/>
+        <c:crossAx val="65263104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1798,7 +1798,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39491456"/>
+        <c:axId val="65263104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1812,7 +1812,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39489920"/>
+        <c:crossAx val="65261568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1836,469 +1836,6 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-MX"/>
-              <a:t>Costo</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'[1]Desviacion de costos'!$C$18:$C$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Planeado</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'[1]Desviacion de costos'!$B$20:$B$27</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>Prospectación</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ventas</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Planeación</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Compras</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Implementación</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Cierre</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Garantia</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Soporte</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'[1]Desviacion de costos'!$C$20:$C$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-15F3-4939-9302-9660B3AF6930}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'[1]Desviacion de costos'!$D$18:$D$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Real </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'[1]Desviacion de costos'!$B$20:$B$27</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>Prospectación</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ventas</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Planeación</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Compras</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Implementación</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Cierre</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Garantia</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Soporte</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'[1]Desviacion de costos'!$D$20:$D$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-15F3-4939-9302-9660B3AF6930}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="110881792"/>
-        <c:axId val="187134720"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="110881792"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187134720"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="187134720"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110881792"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Desviación</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'[1]Desviacion de costos'!$E$18:$E$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Desviación</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'[1]Desviacion de costos'!$B$20:$B$27</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>Prospectación</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ventas</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Planeación</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Compras</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Implementación</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Cierre</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Garantia</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Soporte</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'[1]Desviacion de costos'!$E$20:$E$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4C53-4413-9153-0DEA66086AD7}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="111411584"/>
-        <c:axId val="111413120"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="111411584"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111413120"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="111413120"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111411584"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-MX"/>
@@ -2607,11 +2144,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="39577472"/>
-        <c:axId val="39579008"/>
+        <c:axId val="65312256"/>
+        <c:axId val="65313792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39577472"/>
+        <c:axId val="65312256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2621,7 +2158,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39579008"/>
+        <c:crossAx val="65313792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2629,7 +2166,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39579008"/>
+        <c:axId val="65313792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2643,7 +2180,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39577472"/>
+        <c:crossAx val="65312256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2666,7 +2203,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-MX"/>
@@ -2975,11 +2512,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="39619584"/>
-        <c:axId val="39625472"/>
+        <c:axId val="76651136"/>
+        <c:axId val="76661120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39619584"/>
+        <c:axId val="76651136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2989,7 +2526,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39625472"/>
+        <c:crossAx val="76661120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2997,7 +2534,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39625472"/>
+        <c:axId val="76661120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3011,7 +2548,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39619584"/>
+        <c:crossAx val="76651136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3034,7 +2571,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-MX"/>
@@ -3343,11 +2880,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="39678336"/>
-        <c:axId val="39679872"/>
+        <c:axId val="77090816"/>
+        <c:axId val="77092352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39678336"/>
+        <c:axId val="77090816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3357,7 +2894,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39679872"/>
+        <c:crossAx val="77092352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3365,7 +2902,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39679872"/>
+        <c:axId val="77092352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3379,7 +2916,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39678336"/>
+        <c:crossAx val="77090816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3402,7 +2939,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-MX"/>
@@ -3711,11 +3248,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="39712256"/>
-        <c:axId val="39713792"/>
+        <c:axId val="79316096"/>
+        <c:axId val="79317632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39712256"/>
+        <c:axId val="79316096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3725,7 +3262,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39713792"/>
+        <c:crossAx val="79317632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3733,7 +3270,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39713792"/>
+        <c:axId val="79317632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3747,7 +3284,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39712256"/>
+        <c:crossAx val="79316096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3802,6 +3339,82 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3072401</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2114550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="4 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152401" y="762001"/>
+          <a:ext cx="5253625" cy="2114549"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3257550</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>7239000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2070197</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="6 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5591175" y="819150"/>
+          <a:ext cx="3981450" cy="2013047"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3837,80 +3450,80 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1409700</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>2400300</xdr:rowOff>
+      <xdr:colOff>1981200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>22626</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="3 Gráfico">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="1 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152400" y="952501"/>
+          <a:ext cx="4162425" cy="2432450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>2000251</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>5553075</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>10907</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="4 Gráfico">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="4 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4333876" y="923925"/>
+          <a:ext cx="3981450" cy="2449307"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3950,6 +3563,82 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3851313</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2371725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="2 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152401" y="800101"/>
+          <a:ext cx="6032537" cy="2371724"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4514850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>8315325</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2349279</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="3 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6848475" y="714375"/>
+          <a:ext cx="3800475" cy="2435004"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3985,6 +3674,82 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2007769</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2409825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="2 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152400" y="952500"/>
+          <a:ext cx="4188994" cy="2409825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2031256</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6181725</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="4 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4364881" y="933450"/>
+          <a:ext cx="4150469" cy="2438400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4024,6 +3789,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>790576</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2400301</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2430759</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="2 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="942976" y="762000"/>
+          <a:ext cx="3790950" cy="2430759"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4059,6 +3862,87 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>447676</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1876425</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2346454</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="2 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="600076" y="790575"/>
+          <a:ext cx="3609974" cy="2317879"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2215672</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="1 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="933451"/>
+          <a:ext cx="3457575" cy="2215671"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4201,12 +4085,6 @@
       </sheetData>
       <sheetData sheetId="1">
         <row r="19">
-          <cell r="C19" t="str">
-            <v>Planeado</v>
-          </cell>
-          <cell r="D19" t="str">
-            <v xml:space="preserve">Real </v>
-          </cell>
           <cell r="E19" t="str">
             <v>Desviación</v>
           </cell>
@@ -4214,12 +4092,6 @@
         <row r="20">
           <cell r="B20" t="str">
             <v>Prospectación</v>
-          </cell>
-          <cell r="C20">
-            <v>0</v>
-          </cell>
-          <cell r="D20">
-            <v>0</v>
           </cell>
           <cell r="E20" t="e">
             <v>#DIV/0!</v>
@@ -4229,12 +4101,6 @@
           <cell r="B21" t="str">
             <v>Ventas</v>
           </cell>
-          <cell r="C21">
-            <v>0</v>
-          </cell>
-          <cell r="D21">
-            <v>0</v>
-          </cell>
           <cell r="E21" t="e">
             <v>#DIV/0!</v>
           </cell>
@@ -4242,12 +4108,6 @@
         <row r="22">
           <cell r="B22" t="str">
             <v>Planeación</v>
-          </cell>
-          <cell r="C22">
-            <v>0</v>
-          </cell>
-          <cell r="D22">
-            <v>0</v>
           </cell>
           <cell r="E22" t="e">
             <v>#DIV/0!</v>
@@ -4257,12 +4117,6 @@
           <cell r="B23" t="str">
             <v>Compras</v>
           </cell>
-          <cell r="C23">
-            <v>0</v>
-          </cell>
-          <cell r="D23">
-            <v>0</v>
-          </cell>
           <cell r="E23" t="e">
             <v>#DIV/0!</v>
           </cell>
@@ -4270,12 +4124,6 @@
         <row r="24">
           <cell r="B24" t="str">
             <v>Implementación</v>
-          </cell>
-          <cell r="C24">
-            <v>0</v>
-          </cell>
-          <cell r="D24">
-            <v>0</v>
           </cell>
           <cell r="E24" t="e">
             <v>#DIV/0!</v>
@@ -4285,12 +4133,6 @@
           <cell r="B25" t="str">
             <v>Cierre</v>
           </cell>
-          <cell r="C25">
-            <v>0</v>
-          </cell>
-          <cell r="D25">
-            <v>0</v>
-          </cell>
           <cell r="E25" t="e">
             <v>#DIV/0!</v>
           </cell>
@@ -4298,12 +4140,6 @@
         <row r="26">
           <cell r="B26" t="str">
             <v>Garantia</v>
-          </cell>
-          <cell r="C26">
-            <v>0</v>
-          </cell>
-          <cell r="D26">
-            <v>0</v>
           </cell>
           <cell r="E26" t="e">
             <v>#DIV/0!</v>
@@ -4313,22 +4149,16 @@
           <cell r="B27" t="str">
             <v>Soporte</v>
           </cell>
-          <cell r="C27">
-            <v>0</v>
-          </cell>
-          <cell r="D27">
-            <v>0</v>
-          </cell>
           <cell r="E27" t="e">
             <v>#DIV/0!</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4830,7 +4660,7 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
@@ -4855,7 +4685,7 @@
         <v>Desviación de esfuerzo (%)</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="30" outlineLevel="1">
+    <row r="2" spans="2:3" outlineLevel="1">
       <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
@@ -5191,8 +5021,8 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -5545,8 +5375,8 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -5895,8 +5725,8 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -6247,8 +6077,8 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -6599,8 +6429,8 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -6949,8 +6779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -7179,5 +7009,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
integracion de objetivo de ventas anuales
</commit_message>
<xml_diff>
--- a/Organización/Métricas y monitoreo/Plan_Métricas_aaaa.xlsx
+++ b/Organización/Métricas y monitoreo/Plan_Métricas_aaaa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-1365" yWindow="300" windowWidth="16605" windowHeight="9435" tabRatio="971" activeTab="2"/>
+    <workbookView xWindow="-1365" yWindow="300" windowWidth="16605" windowHeight="9435" tabRatio="971" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Objetivos de Medición" sheetId="1" r:id="rId1"/>
@@ -14,8 +14,12 @@
     <sheet name="Apego a Productos " sheetId="17" r:id="rId5"/>
     <sheet name="Apego a Auditorias Fisicas" sheetId="18" r:id="rId6"/>
     <sheet name="Apego a Auditorias Funcionales" sheetId="19" r:id="rId7"/>
-    <sheet name="Índice de Satisfacción" sheetId="20" r:id="rId8"/>
+    <sheet name="Crecimiento anual de ventas" sheetId="21" r:id="rId8"/>
+    <sheet name="Índice de Satisfacción" sheetId="20" r:id="rId9"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId10"/>
+  </externalReferences>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="140">
   <si>
     <t>Objetivos/Necesidades de Negocio y  Medición</t>
   </si>
@@ -248,9 +252,6 @@
   </si>
   <si>
     <t xml:space="preserve">¿Cuál es la deviacion del costo?                                                                                                                                     </t>
-  </si>
-  <si>
-    <t>Desviación de esfuerzo (%)</t>
   </si>
   <si>
     <t>¿Cuál es el porcentaje de apego a proceso del proyecto?</t>
@@ -293,9 +294,6 @@
   </si>
   <si>
     <t>Se analiza con direccion para tomar medidas inmeditas para corregir la desviacion y considerar actualizar la estimación del servicio</t>
-  </si>
-  <si>
-    <t>Desviación de costo (%)</t>
   </si>
   <si>
     <t>Que el índice de satisfacción sea menor a 70%</t>
@@ -425,6 +423,57 @@
   </si>
   <si>
     <t>Si la desvacion es mayor al 15% y menor o igual a 30%</t>
+  </si>
+  <si>
+    <t>Quincenal</t>
+  </si>
+  <si>
+    <t>Crear plan de acción para aumentar el porcentaje de cumplimiento en ventas.</t>
+  </si>
+  <si>
+    <t>Crear un plan de acción en base a los malos resultados obtenidos.</t>
+  </si>
+  <si>
+    <t>Desviación de esfuerzo</t>
+  </si>
+  <si>
+    <t>Desviación de costo</t>
+  </si>
+  <si>
+    <t>Obtener un crecimiento anual del 40% representado por un total de 2,424,000</t>
+  </si>
+  <si>
+    <t>Crecimiento anual de ventas</t>
+  </si>
+  <si>
+    <t>Que el índice de ventas sea menor o igual a 80%</t>
+  </si>
+  <si>
+    <t>Que el índice de ventas sea menor que 90% y mayor o igual a 81%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que el índice de ventas sea mayor o igual a 91% </t>
+  </si>
+  <si>
+    <t>Total esperado anual</t>
+  </si>
+  <si>
+    <t>Total obtenido quincenal</t>
+  </si>
+  <si>
+    <t>Conocer el apegó a la meta de ventas anuales en la empresa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Se esta cumpliendo la cuota establecida de forma quincenal?                                             </t>
+  </si>
+  <si>
+    <t>Hacer la sumatoria total de ventas en la quincena por empleado, para ello tomar los datos almacenados en el documento control de ventas, generar el calculo acorde a la formula definida y registrar los resultados en el concentrado de métricas, pestaña ventas, a su vez  integrar los resultados obtenidos en forma global y tambien desglozarlo por empleado.</t>
+  </si>
+  <si>
+    <t>Acumulado Total</t>
+  </si>
+  <si>
+    <t>Venta por empleado = (sumatoria de ventas por empleado)                                                                         Venta quincenal =  suma de ventas por empleado</t>
   </si>
 </sst>
 </file>
@@ -797,7 +846,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1"/>
@@ -920,6 +969,21 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -941,15 +1005,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1000,6 +1055,30 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1401,11 +1480,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="56126080"/>
-        <c:axId val="56140160"/>
+        <c:axId val="57436800"/>
+        <c:axId val="57450880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="56126080"/>
+        <c:axId val="57436800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1415,7 +1494,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56140160"/>
+        <c:crossAx val="57450880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1423,7 +1502,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56140160"/>
+        <c:axId val="57450880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1437,7 +1516,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56126080"/>
+        <c:crossAx val="57436800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1773,11 +1852,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="39678720"/>
-        <c:axId val="39680256"/>
+        <c:axId val="79856384"/>
+        <c:axId val="79857920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39678720"/>
+        <c:axId val="79856384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1787,7 +1866,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39680256"/>
+        <c:crossAx val="79857920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1795,7 +1874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39680256"/>
+        <c:axId val="79857920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1809,7 +1888,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39678720"/>
+        <c:crossAx val="79856384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2141,11 +2220,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="39512320"/>
-        <c:axId val="39514112"/>
+        <c:axId val="57080064"/>
+        <c:axId val="57085952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39512320"/>
+        <c:axId val="57080064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2155,7 +2234,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39514112"/>
+        <c:crossAx val="57085952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2163,7 +2242,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39514112"/>
+        <c:axId val="57085952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2177,7 +2256,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39512320"/>
+        <c:crossAx val="57080064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2509,11 +2588,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="39624064"/>
-        <c:axId val="39625856"/>
+        <c:axId val="57126272"/>
+        <c:axId val="57132160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39624064"/>
+        <c:axId val="57126272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2523,7 +2602,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39625856"/>
+        <c:crossAx val="57132160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2531,7 +2610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39625856"/>
+        <c:axId val="57132160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2545,7 +2624,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39624064"/>
+        <c:crossAx val="57126272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2877,11 +2956,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="39778944"/>
-        <c:axId val="39788928"/>
+        <c:axId val="79952128"/>
+        <c:axId val="79962112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39778944"/>
+        <c:axId val="79952128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2891,7 +2970,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39788928"/>
+        <c:crossAx val="79962112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2899,7 +2978,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39788928"/>
+        <c:axId val="79962112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2913,7 +2992,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39778944"/>
+        <c:crossAx val="79952128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3245,11 +3324,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="39833600"/>
-        <c:axId val="39835136"/>
+        <c:axId val="80007168"/>
+        <c:axId val="80008704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39833600"/>
+        <c:axId val="80007168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3259,7 +3338,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39835136"/>
+        <c:crossAx val="80008704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3267,7 +3346,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39835136"/>
+        <c:axId val="80008704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3281,7 +3360,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39833600"/>
+        <c:crossAx val="80007168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3907,6 +3986,87 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3295651</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1676736</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="19 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="771525"/>
+          <a:ext cx="3295650" cy="1667211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>723901</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4314825</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1779693</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="20 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4619626" y="762000"/>
+          <a:ext cx="3590924" cy="1779693"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
@@ -3943,6 +4103,92 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Desviacion de esfuerzo"/>
+      <sheetName val="Desviacion de costos"/>
+      <sheetName val="Apego a Procesos"/>
+      <sheetName val="Apego a Productos"/>
+      <sheetName val="Física"/>
+      <sheetName val="Funcional"/>
+      <sheetName val="Crecimiento anual de ventas"/>
+      <sheetName val="Indice de Satisfacción"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6">
+        <row r="13">
+          <cell r="G13" t="str">
+            <v>Monto Total</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14" t="str">
+            <v>Planeado</v>
+          </cell>
+          <cell r="C14" t="str">
+            <v xml:space="preserve">Real </v>
+          </cell>
+          <cell r="G14" t="str">
+            <v>Planeado</v>
+          </cell>
+          <cell r="H14" t="str">
+            <v xml:space="preserve">Real </v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>Periodo</v>
+          </cell>
+          <cell r="B15">
+            <v>12345</v>
+          </cell>
+          <cell r="C15">
+            <v>11234</v>
+          </cell>
+          <cell r="G15">
+            <v>2424000</v>
+          </cell>
+          <cell r="H15">
+            <v>11234</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>Oriana</v>
+          </cell>
+          <cell r="B16">
+            <v>6172.5</v>
+          </cell>
+          <cell r="C16">
+            <v>6123</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>Marisol</v>
+          </cell>
+          <cell r="B17">
+            <v>6172.5</v>
+          </cell>
+          <cell r="C17">
+            <v>5234</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4235,10 +4481,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4252,13 +4498,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75">
       <c r="A1" s="21"/>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:7">
@@ -4270,22 +4516,22 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="24.6" customHeight="1">
-      <c r="B3" s="63" t="s">
-        <v>122</v>
+      <c r="B3" s="57" t="s">
+        <v>120</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="11" customFormat="1" ht="21" customHeight="1">
-      <c r="B4" s="63"/>
+      <c r="B4" s="57"/>
       <c r="C4" s="23" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="B5" s="63" t="s">
-        <v>97</v>
+      <c r="B5" s="57" t="s">
+        <v>95</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>22</v>
@@ -4294,135 +4540,143 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="22"/>
-      <c r="B6" s="63"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" s="57"/>
+      <c r="C7" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" s="57"/>
+      <c r="C8" s="23" t="s">
         <v>79</v>
-      </c>
-      <c r="D6" s="22"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" s="63"/>
-      <c r="C7" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="22"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="63"/>
-      <c r="C8" s="23" t="s">
-        <v>80</v>
       </c>
       <c r="D8" s="22"/>
     </row>
     <row r="9" spans="1:7" ht="30">
       <c r="B9" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="18.75">
-      <c r="A11" s="21"/>
-      <c r="B11" s="59" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="11" customFormat="1" ht="30">
+      <c r="B10" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="18.75">
+      <c r="A12" s="21"/>
+      <c r="B12" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" s="5" customFormat="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="64"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="66"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1">
       <c r="A13" s="3"/>
-      <c r="B13" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="56"/>
-      <c r="E13" s="57" t="s">
-        <v>110</v>
+      <c r="B13" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58" t="s">
+        <v>10</v>
       </c>
       <c r="F13" s="58"/>
-    </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" ht="19.149999999999999" customHeight="1">
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1">
       <c r="A14" s="3"/>
       <c r="B14" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="61"/>
+      <c r="E14" s="62" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" s="63"/>
+    </row>
+    <row r="15" spans="1:7" s="5" customFormat="1" ht="19.149999999999999" customHeight="1">
+      <c r="A15" s="3"/>
+      <c r="B15" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="54" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="F14" s="58"/>
-    </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" s="5" customFormat="1" ht="26.25" customHeight="1">
+      <c r="C15" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="60"/>
+      <c r="E15" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="63"/>
+    </row>
+    <row r="16" spans="1:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A16" s="3"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:7" s="5" customFormat="1">
+    <row r="17" spans="1:7" s="5" customFormat="1" ht="26.25" customHeight="1">
       <c r="A17" s="3"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" ht="18.75">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+    <row r="18" spans="1:7" s="5" customFormat="1">
+      <c r="A18" s="3"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" s="2" customFormat="1" ht="18.75">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C15:D17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B12:F12"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C14:D16"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="B11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4441,8 +4695,8 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4463,7 +4717,7 @@
       </c>
       <c r="C1" s="29" t="str">
         <f>'Objetivos de Medición'!C3</f>
-        <v>Desviación de esfuerzo (%)</v>
+        <v>Desviación de esfuerzo</v>
       </c>
     </row>
     <row r="2" spans="2:3" outlineLevel="1">
@@ -4471,7 +4725,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="2:3" outlineLevel="1">
@@ -4483,20 +4737,20 @@
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="68"/>
+      <c r="C4" s="70"/>
     </row>
     <row r="5" spans="2:3" ht="187.15" customHeight="1" outlineLevel="1">
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
     </row>
     <row r="6" spans="2:3" outlineLevel="1">
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="67"/>
+      <c r="C6" s="69"/>
     </row>
     <row r="7" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B7" s="29" t="s">
@@ -4510,35 +4764,35 @@
       <c r="B8" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="70" t="s">
-        <v>95</v>
+      <c r="C8" s="72" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
       <c r="B9" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="70"/>
+      <c r="C9" s="72"/>
     </row>
     <row r="10" spans="2:3" outlineLevel="1">
       <c r="B10" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="31" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="11" spans="2:3" outlineLevel="1">
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="69"/>
     </row>
     <row r="12" spans="2:3" ht="48" customHeight="1" outlineLevel="1">
-      <c r="B12" s="66" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" s="66"/>
+      <c r="B12" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="68"/>
     </row>
     <row r="13" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B13" s="29" t="s">
@@ -4549,16 +4803,18 @@
       </c>
     </row>
     <row r="14" spans="2:3" outlineLevel="1">
-      <c r="B14" s="30"/>
+      <c r="B14" s="54" t="s">
+        <v>123</v>
+      </c>
       <c r="C14" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:3" outlineLevel="1">
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="67"/>
+      <c r="C15" s="69"/>
     </row>
     <row r="16" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B16" s="29" t="s">
@@ -4569,7 +4825,9 @@
       </c>
     </row>
     <row r="17" spans="2:3" outlineLevel="1">
-      <c r="B17" s="30"/>
+      <c r="B17" s="30" t="s">
+        <v>123</v>
+      </c>
       <c r="C17" s="32" t="s">
         <v>21</v>
       </c>
@@ -4583,26 +4841,28 @@
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
-      <c r="B19" s="30"/>
+      <c r="B19" s="54" t="s">
+        <v>33</v>
+      </c>
       <c r="C19" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
-      <c r="B20" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="67"/>
+      <c r="B20" s="69" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="69"/>
     </row>
     <row r="21" spans="2:3" s="18" customFormat="1" outlineLevel="1">
-      <c r="B21" s="65" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" s="65"/>
+      <c r="B21" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="67"/>
     </row>
     <row r="22" spans="2:3" outlineLevel="1">
       <c r="B22" s="33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>70</v>
@@ -4610,7 +4870,7 @@
     </row>
     <row r="23" spans="2:3" ht="30">
       <c r="B23" s="34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>71</v>
@@ -4618,10 +4878,10 @@
     </row>
     <row r="24" spans="2:3" ht="30">
       <c r="B24" s="35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -4802,8 +5062,8 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView showGridLines="0" topLeftCell="A12" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4824,7 +5084,7 @@
       </c>
       <c r="C1" s="29" t="str">
         <f>'Objetivos de Medición'!C4</f>
-        <v>Desviación de costo (%)</v>
+        <v>Desviación de costo</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="30" outlineLevel="1">
@@ -4844,20 +5104,20 @@
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="68"/>
+      <c r="C4" s="70"/>
     </row>
     <row r="5" spans="2:3" ht="190.15" customHeight="1" outlineLevel="1">
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
     </row>
     <row r="6" spans="2:3" outlineLevel="1">
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="67"/>
+      <c r="C6" s="69"/>
     </row>
     <row r="7" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B7" s="29" t="s">
@@ -4871,35 +5131,35 @@
       <c r="B8" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="70" t="s">
-        <v>96</v>
+      <c r="C8" s="72" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
       <c r="B9" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="70"/>
+      <c r="C9" s="72"/>
     </row>
     <row r="10" spans="2:3" outlineLevel="1">
       <c r="B10" s="30" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="2:3" outlineLevel="1">
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="69"/>
     </row>
     <row r="12" spans="2:3" ht="63.75" customHeight="1" outlineLevel="1">
-      <c r="B12" s="66" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12" s="66"/>
+      <c r="B12" s="68" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="68"/>
     </row>
     <row r="13" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B13" s="29" t="s">
@@ -4910,16 +5170,18 @@
       </c>
     </row>
     <row r="14" spans="2:3" outlineLevel="1">
-      <c r="B14" s="30"/>
+      <c r="B14" s="54" t="s">
+        <v>123</v>
+      </c>
       <c r="C14" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:3" outlineLevel="1">
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="67"/>
+      <c r="C15" s="69"/>
     </row>
     <row r="16" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B16" s="29" t="s">
@@ -4930,7 +5192,9 @@
       </c>
     </row>
     <row r="17" spans="2:3" outlineLevel="1">
-      <c r="B17" s="30"/>
+      <c r="B17" s="54" t="s">
+        <v>123</v>
+      </c>
       <c r="C17" s="32" t="s">
         <v>21</v>
       </c>
@@ -4944,20 +5208,22 @@
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
-      <c r="B19" s="30"/>
+      <c r="B19" s="54" t="s">
+        <v>33</v>
+      </c>
       <c r="C19" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
-      <c r="B20" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="67"/>
+      <c r="B20" s="69" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="69"/>
     </row>
     <row r="21" spans="2:3" outlineLevel="1">
       <c r="B21" s="33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>70</v>
@@ -4965,7 +5231,7 @@
     </row>
     <row r="22" spans="2:3" ht="30">
       <c r="B22" s="34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>71</v>
@@ -4973,10 +5239,10 @@
     </row>
     <row r="23" spans="2:3" ht="30">
       <c r="B23" s="35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -5156,8 +5422,8 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -5192,24 +5458,24 @@
         <v>69</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="68"/>
+      <c r="C4" s="70"/>
     </row>
     <row r="5" spans="2:3" ht="187.9" customHeight="1" outlineLevel="1">
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
     </row>
     <row r="6" spans="2:3" outlineLevel="1">
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="67"/>
+      <c r="C6" s="69"/>
     </row>
     <row r="7" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B7" s="29" t="s">
@@ -5223,33 +5489,33 @@
       <c r="B8" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="71" t="s">
-        <v>108</v>
+      <c r="C8" s="73" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
       <c r="B9" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="72"/>
+        <v>102</v>
+      </c>
+      <c r="C9" s="74"/>
     </row>
     <row r="10" spans="2:3" ht="30" outlineLevel="1">
       <c r="B10" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="73"/>
+        <v>103</v>
+      </c>
+      <c r="C10" s="75"/>
     </row>
     <row r="11" spans="2:3" outlineLevel="1">
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="69"/>
     </row>
     <row r="12" spans="2:3" ht="37.5" customHeight="1" outlineLevel="1">
-      <c r="B12" s="66" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="66"/>
+      <c r="B12" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="68"/>
     </row>
     <row r="13" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B13" s="29" t="s">
@@ -5260,16 +5526,18 @@
       </c>
     </row>
     <row r="14" spans="2:3" outlineLevel="1">
-      <c r="B14" s="30"/>
+      <c r="B14" s="54" t="s">
+        <v>123</v>
+      </c>
       <c r="C14" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:3" outlineLevel="1">
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="67"/>
+      <c r="C15" s="69"/>
     </row>
     <row r="16" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B16" s="29" t="s">
@@ -5280,7 +5548,9 @@
       </c>
     </row>
     <row r="17" spans="2:3" outlineLevel="1">
-      <c r="B17" s="30"/>
+      <c r="B17" s="54" t="s">
+        <v>123</v>
+      </c>
       <c r="C17" s="32" t="s">
         <v>45</v>
       </c>
@@ -5294,23 +5564,25 @@
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
-      <c r="B19" s="30"/>
+      <c r="B19" s="54" t="s">
+        <v>33</v>
+      </c>
       <c r="C19" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
-      <c r="B20" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="67"/>
+      <c r="B20" s="69" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="69"/>
     </row>
     <row r="21" spans="2:3" outlineLevel="1">
       <c r="B21" s="40" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="2:3">
@@ -5318,7 +5590,7 @@
         <v>43</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="2:3">
@@ -5326,7 +5598,7 @@
         <v>44</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -5506,8 +5778,8 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -5536,7 +5808,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="2:3" outlineLevel="1">
@@ -5544,24 +5816,24 @@
         <v>69</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="68"/>
+      <c r="C4" s="70"/>
     </row>
     <row r="5" spans="2:3" ht="190.9" customHeight="1" outlineLevel="1">
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
     </row>
     <row r="6" spans="2:3" outlineLevel="1">
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="67"/>
+      <c r="C6" s="69"/>
     </row>
     <row r="7" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B7" s="29" t="s">
@@ -5575,33 +5847,33 @@
       <c r="B8" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="74" t="s">
-        <v>106</v>
+      <c r="C8" s="76" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
       <c r="B9" s="52" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="75"/>
+        <v>102</v>
+      </c>
+      <c r="C9" s="77"/>
     </row>
     <row r="10" spans="2:3" ht="30" outlineLevel="1">
       <c r="B10" s="52" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="76"/>
+        <v>103</v>
+      </c>
+      <c r="C10" s="78"/>
     </row>
     <row r="11" spans="2:3" outlineLevel="1">
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="69"/>
     </row>
     <row r="12" spans="2:3" ht="39.75" customHeight="1" outlineLevel="1">
-      <c r="B12" s="66" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="66"/>
+      <c r="B12" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="68"/>
     </row>
     <row r="13" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B13" s="29" t="s">
@@ -5612,16 +5884,18 @@
       </c>
     </row>
     <row r="14" spans="2:3" outlineLevel="1">
-      <c r="B14" s="30"/>
+      <c r="B14" s="54" t="s">
+        <v>123</v>
+      </c>
       <c r="C14" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:3" outlineLevel="1">
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="67"/>
+      <c r="C15" s="69"/>
     </row>
     <row r="16" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B16" s="29" t="s">
@@ -5632,7 +5906,9 @@
       </c>
     </row>
     <row r="17" spans="2:3" outlineLevel="1">
-      <c r="B17" s="30"/>
+      <c r="B17" s="54" t="s">
+        <v>123</v>
+      </c>
       <c r="C17" s="32" t="s">
         <v>46</v>
       </c>
@@ -5646,23 +5922,25 @@
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
-      <c r="B19" s="30"/>
+      <c r="B19" s="54" t="s">
+        <v>33</v>
+      </c>
       <c r="C19" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
-      <c r="B20" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="67"/>
+      <c r="B20" s="69" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="69"/>
     </row>
     <row r="21" spans="2:3" outlineLevel="1">
       <c r="B21" s="41" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="2:3">
@@ -5670,7 +5948,7 @@
         <v>43</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="2:3">
@@ -5678,7 +5956,7 @@
         <v>44</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -5858,8 +6136,8 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -5896,24 +6174,24 @@
         <v>69</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="68"/>
+      <c r="C4" s="70"/>
     </row>
     <row r="5" spans="2:3" ht="192.6" customHeight="1" outlineLevel="1">
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
     </row>
     <row r="6" spans="2:3" outlineLevel="1">
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="67"/>
+      <c r="C6" s="69"/>
     </row>
     <row r="7" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B7" s="29" t="s">
@@ -5927,33 +6205,33 @@
       <c r="B8" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="71" t="s">
-        <v>107</v>
+      <c r="C8" s="73" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
       <c r="B9" s="52" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="72"/>
+        <v>102</v>
+      </c>
+      <c r="C9" s="74"/>
     </row>
     <row r="10" spans="2:3" ht="30" outlineLevel="1">
       <c r="B10" s="52" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="73"/>
+        <v>103</v>
+      </c>
+      <c r="C10" s="75"/>
     </row>
     <row r="11" spans="2:3" outlineLevel="1">
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="69"/>
     </row>
     <row r="12" spans="2:3" ht="46.9" customHeight="1" outlineLevel="1">
-      <c r="B12" s="66" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" s="66"/>
+      <c r="B12" s="68" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="68"/>
     </row>
     <row r="13" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B13" s="29" t="s">
@@ -5964,16 +6242,18 @@
       </c>
     </row>
     <row r="14" spans="2:3" outlineLevel="1">
-      <c r="B14" s="30"/>
+      <c r="B14" s="54" t="s">
+        <v>123</v>
+      </c>
       <c r="C14" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:3" outlineLevel="1">
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="67"/>
+      <c r="C15" s="69"/>
     </row>
     <row r="16" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B16" s="29" t="s">
@@ -5984,7 +6264,9 @@
       </c>
     </row>
     <row r="17" spans="2:3" outlineLevel="1">
-      <c r="B17" s="30"/>
+      <c r="B17" s="54" t="s">
+        <v>123</v>
+      </c>
       <c r="C17" s="32" t="s">
         <v>46</v>
       </c>
@@ -5998,23 +6280,25 @@
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
-      <c r="B19" s="30"/>
+      <c r="B19" s="54" t="s">
+        <v>33</v>
+      </c>
       <c r="C19" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
-      <c r="B20" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="67"/>
+      <c r="B20" s="69" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="69"/>
     </row>
     <row r="21" spans="2:3" outlineLevel="1">
       <c r="B21" s="41" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="2:3">
@@ -6022,7 +6306,7 @@
         <v>43</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="2:3">
@@ -6030,7 +6314,7 @@
         <v>44</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -6210,8 +6494,8 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -6252,20 +6536,20 @@
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="68"/>
+      <c r="C4" s="70"/>
     </row>
     <row r="5" spans="2:3" ht="187.15" customHeight="1" outlineLevel="1">
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
     </row>
     <row r="6" spans="2:3" outlineLevel="1">
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="67"/>
+      <c r="C6" s="69"/>
     </row>
     <row r="7" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B7" s="29" t="s">
@@ -6279,33 +6563,33 @@
       <c r="B8" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="71" t="s">
-        <v>109</v>
+      <c r="C8" s="73" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
       <c r="B9" s="52" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="72"/>
+        <v>102</v>
+      </c>
+      <c r="C9" s="74"/>
     </row>
     <row r="10" spans="2:3" ht="30" outlineLevel="1">
       <c r="B10" s="52" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="73"/>
+        <v>103</v>
+      </c>
+      <c r="C10" s="75"/>
     </row>
     <row r="11" spans="2:3" outlineLevel="1">
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="69"/>
     </row>
     <row r="12" spans="2:3" ht="45.6" customHeight="1" outlineLevel="1">
-      <c r="B12" s="66" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" s="66"/>
+      <c r="B12" s="68" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="68"/>
     </row>
     <row r="13" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B13" s="29" t="s">
@@ -6316,16 +6600,18 @@
       </c>
     </row>
     <row r="14" spans="2:3" outlineLevel="1">
-      <c r="B14" s="30"/>
+      <c r="B14" s="54" t="s">
+        <v>123</v>
+      </c>
       <c r="C14" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:3" outlineLevel="1">
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="67"/>
+      <c r="C15" s="69"/>
     </row>
     <row r="16" spans="2:3" ht="15" customHeight="1" outlineLevel="1">
       <c r="B16" s="29" t="s">
@@ -6336,7 +6622,9 @@
       </c>
     </row>
     <row r="17" spans="2:3" outlineLevel="1">
-      <c r="B17" s="30"/>
+      <c r="B17" s="54" t="s">
+        <v>123</v>
+      </c>
       <c r="C17" s="32" t="s">
         <v>46</v>
       </c>
@@ -6350,23 +6638,25 @@
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
-      <c r="B19" s="30"/>
+      <c r="B19" s="54" t="s">
+        <v>33</v>
+      </c>
       <c r="C19" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
-      <c r="B20" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="67"/>
+      <c r="B20" s="69" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="69"/>
     </row>
     <row r="21" spans="2:3" outlineLevel="1">
       <c r="B21" s="41" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="2:3">
@@ -6374,7 +6664,7 @@
         <v>43</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="2:3">
@@ -6382,7 +6672,7 @@
         <v>44</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -6558,10 +6848,205 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="58.42578125" customWidth="1"/>
+    <col min="2" max="2" width="76" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="84" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="80" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="80"/>
+    </row>
+    <row r="5" spans="1:2" ht="141" customHeight="1">
+      <c r="A5" s="85"/>
+      <c r="B5" s="85"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="80"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="11" customFormat="1">
+      <c r="A8" s="86" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="87" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="11" customFormat="1">
+      <c r="A9" s="86" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="88"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="89"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="80" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="80"/>
+    </row>
+    <row r="12" spans="1:2" ht="45.75" customHeight="1">
+      <c r="A12" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="91"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="54" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="80" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="80"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="55" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="54" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30">
+      <c r="A18" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="55" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="80"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" s="54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28.5">
+      <c r="A22" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A15:B15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6597,20 +7082,20 @@
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="79"/>
+      <c r="B4" s="81"/>
     </row>
     <row r="5" spans="1:21" ht="184.5" customHeight="1">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80"/>
+      <c r="A5" s="82"/>
+      <c r="B5" s="82"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="78"/>
+      <c r="B6" s="80"/>
       <c r="Q6" s="11" t="s">
         <v>51</v>
       </c>
@@ -6682,16 +7167,16 @@
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="78"/>
+      <c r="B9" s="80"/>
     </row>
     <row r="10" spans="1:21" ht="61.5" customHeight="1">
-      <c r="A10" s="81" t="s">
-        <v>119</v>
-      </c>
-      <c r="B10" s="81"/>
+      <c r="A10" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="83"/>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="48" t="s">
@@ -6702,16 +7187,18 @@
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="30"/>
+      <c r="A12" s="54" t="s">
+        <v>123</v>
+      </c>
       <c r="B12" s="30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="78"/>
+      <c r="B13" s="80"/>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="48" t="s">
@@ -6722,7 +7209,9 @@
       </c>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="30"/>
+      <c r="A15" s="54" t="s">
+        <v>123</v>
+      </c>
       <c r="B15" s="30" t="s">
         <v>63</v>
       </c>
@@ -6736,26 +7225,28 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="30"/>
+      <c r="A17" s="30" t="s">
+        <v>33</v>
+      </c>
       <c r="B17" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="78" t="s">
-        <v>101</v>
-      </c>
-      <c r="B18" s="78"/>
+      <c r="A18" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="80"/>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="77" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19" s="77"/>
+      <c r="A19" s="79" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="79"/>
     </row>
     <row r="20" spans="1:2" ht="28.5">
       <c r="A20" s="49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>64</v>
@@ -6763,15 +7254,15 @@
     </row>
     <row r="21" spans="1:2" ht="28.5">
       <c r="A21" s="50" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="51" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B22" s="30" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
cambios en revision de aufitoria y reporte de proyecto multiples
</commit_message>
<xml_diff>
--- a/Organización/Métricas y monitoreo/Plan_Métricas_aaaa.xlsx
+++ b/Organización/Métricas y monitoreo/Plan_Métricas_aaaa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Objetivos de Medición" sheetId="1" state="visible" r:id="rId2"/>
@@ -198,19 +198,19 @@
     <t>El análisis se hara en base a la grafica de Desviación</t>
   </si>
   <si>
-    <t>Si la desviacion es de 0% a 15%</t>
+    <t>Si la desviacion es de 0% a 100%</t>
   </si>
   <si>
     <t>Se continua con el seguimiento</t>
   </si>
   <si>
-    <t>Si la desvacion es mayor al 15% y menor o igual a 30%</t>
+    <t>Si la desvacion es menor a 0% y mayor o igual a -10%</t>
   </si>
   <si>
     <t>Se monitorea y analiza con dirección, se toman acciones para reducir la desviación</t>
   </si>
   <si>
-    <t>Si la desviación es menor que 0 o Si la desviacion es mayor a 30% </t>
+    <t>Si la desviación es menor que -10% </t>
   </si>
   <si>
     <t>Se analiza con direccion para tomar medidas inmeditas para corregir la desviacion y considerar actualizar la estimación del servicio</t>
@@ -1320,11 +1320,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="74157567"/>
-        <c:axId val="72440041"/>
+        <c:axId val="88704240"/>
+        <c:axId val="72829875"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74157567"/>
+        <c:axId val="88704240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1341,14 +1341,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="72440041"/>
+        <c:crossAx val="72829875"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72440041"/>
+        <c:axId val="72829875"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1398,7 +1398,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="74157567"/>
+        <c:crossAx val="88704240"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -1739,11 +1739,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="15829809"/>
-        <c:axId val="82616405"/>
+        <c:axId val="95742415"/>
+        <c:axId val="29894614"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="15829809"/>
+        <c:axId val="95742415"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1760,14 +1760,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82616405"/>
+        <c:crossAx val="29894614"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82616405"/>
+        <c:axId val="29894614"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1817,7 +1817,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="15829809"/>
+        <c:crossAx val="95742415"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -2164,11 +2164,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="79803306"/>
-        <c:axId val="20112678"/>
+        <c:axId val="50141967"/>
+        <c:axId val="98914208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79803306"/>
+        <c:axId val="50141967"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2185,14 +2185,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="20112678"/>
+        <c:crossAx val="98914208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20112678"/>
+        <c:axId val="98914208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2242,7 +2242,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="79803306"/>
+        <c:crossAx val="50141967"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -2589,11 +2589,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="74789328"/>
-        <c:axId val="80572125"/>
+        <c:axId val="92569714"/>
+        <c:axId val="79222930"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74789328"/>
+        <c:axId val="92569714"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2610,14 +2610,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="80572125"/>
+        <c:crossAx val="79222930"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80572125"/>
+        <c:axId val="79222930"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2667,7 +2667,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="74789328"/>
+        <c:crossAx val="92569714"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -3014,11 +3014,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="2654977"/>
-        <c:axId val="68330409"/>
+        <c:axId val="27118907"/>
+        <c:axId val="92958151"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2654977"/>
+        <c:axId val="27118907"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3035,14 +3035,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="68330409"/>
+        <c:crossAx val="92958151"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68330409"/>
+        <c:axId val="92958151"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3092,7 +3092,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2654977"/>
+        <c:crossAx val="27118907"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -3439,11 +3439,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="58572827"/>
-        <c:axId val="86884965"/>
+        <c:axId val="49683211"/>
+        <c:axId val="78625393"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58572827"/>
+        <c:axId val="49683211"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3460,14 +3460,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="86884965"/>
+        <c:crossAx val="78625393"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86884965"/>
+        <c:axId val="78625393"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3517,7 +3517,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="58572827"/>
+        <c:crossAx val="49683211"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -3552,15 +3552,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>309600</xdr:colOff>
+      <xdr:colOff>336600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>194400</xdr:colOff>
+      <xdr:colOff>221040</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>139680</xdr:rowOff>
+      <xdr:rowOff>173520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3568,8 +3568,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="43924320" y="9384120"/>
-        <a:ext cx="5981040" cy="2884680"/>
+        <a:off x="43951320" y="9375120"/>
+        <a:ext cx="5980680" cy="2884320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3582,15 +3582,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3152160</xdr:colOff>
+      <xdr:colOff>3178800</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2086560</xdr:rowOff>
+      <xdr:rowOff>2077200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3603,8 +3603,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="284040" y="734760"/>
-          <a:ext cx="5979960" cy="2113560"/>
+          <a:off x="311040" y="725760"/>
+          <a:ext cx="5979600" cy="2113200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3619,15 +3619,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3338640</xdr:colOff>
+      <xdr:colOff>3365640</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>30240</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7319160</xdr:colOff>
+      <xdr:colOff>7345800</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2042280</xdr:rowOff>
+      <xdr:rowOff>2032920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3640,8 +3640,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6450480" y="792000"/>
-          <a:ext cx="3980520" cy="2012040"/>
+          <a:off x="6477480" y="783000"/>
+          <a:ext cx="3980160" cy="2011680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3661,15 +3661,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>258840</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>189000</xdr:rowOff>
+      <xdr:colOff>285840</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>32760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>232200</xdr:colOff>
+      <xdr:colOff>258840</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>111960</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3677,8 +3677,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="43111080" y="9890280"/>
-        <a:ext cx="8101440" cy="3351960"/>
+        <a:off x="43138080" y="9881280"/>
+        <a:ext cx="8101080" cy="3351600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3691,15 +3691,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2061000</xdr:colOff>
+      <xdr:colOff>2087640</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2409480</xdr:rowOff>
+      <xdr:rowOff>2400120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3712,8 +3712,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="284040" y="925200"/>
-          <a:ext cx="4888800" cy="2436480"/>
+          <a:off x="311040" y="916200"/>
+          <a:ext cx="4888440" cy="2436120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3728,15 +3728,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2081160</xdr:colOff>
+      <xdr:colOff>2108160</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>135000</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>99000</xdr:colOff>
+      <xdr:colOff>125640</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2397960</xdr:rowOff>
+      <xdr:rowOff>2388600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3749,8 +3749,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5193000" y="896760"/>
-          <a:ext cx="5969520" cy="2453400"/>
+          <a:off x="5220000" y="887760"/>
+          <a:ext cx="5969160" cy="2453040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3770,15 +3770,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>309600</xdr:colOff>
+      <xdr:colOff>336600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>111240</xdr:rowOff>
+      <xdr:rowOff>102240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>194400</xdr:colOff>
+      <xdr:colOff>221040</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3786,8 +3786,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="45423720" y="9107640"/>
-        <a:ext cx="5980680" cy="2885040"/>
+        <a:off x="45450720" y="9098640"/>
+        <a:ext cx="5980320" cy="2884680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3800,15 +3800,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3931200</xdr:colOff>
+      <xdr:colOff>3957840</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2343600</xdr:rowOff>
+      <xdr:rowOff>2334240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3821,8 +3821,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="284040" y="772920"/>
-          <a:ext cx="6759000" cy="2370600"/>
+          <a:off x="311040" y="763920"/>
+          <a:ext cx="6758640" cy="2370240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3837,15 +3837,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4595760</xdr:colOff>
+      <xdr:colOff>4622760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>77760</xdr:rowOff>
+      <xdr:rowOff>68760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>8395200</xdr:colOff>
+      <xdr:colOff>8421840</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2321280</xdr:rowOff>
+      <xdr:rowOff>2311920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3858,8 +3858,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7707600" y="687240"/>
-          <a:ext cx="3799440" cy="2433960"/>
+          <a:off x="7734600" y="678240"/>
+          <a:ext cx="3799080" cy="2433600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3879,15 +3879,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>309600</xdr:colOff>
+      <xdr:colOff>336600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>111240</xdr:rowOff>
+      <xdr:rowOff>102240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>194400</xdr:colOff>
+      <xdr:colOff>221040</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3895,8 +3895,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="42463800" y="9326880"/>
-        <a:ext cx="5981040" cy="2884680"/>
+        <a:off x="42490800" y="9317880"/>
+        <a:ext cx="5980680" cy="2884320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3909,15 +3909,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2087640</xdr:colOff>
+      <xdr:colOff>2114280</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2381760</xdr:rowOff>
+      <xdr:rowOff>2372400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3930,8 +3930,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="284040" y="925200"/>
-          <a:ext cx="4915440" cy="2408760"/>
+          <a:off x="311040" y="916200"/>
+          <a:ext cx="4915080" cy="2408400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3946,15 +3946,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2112120</xdr:colOff>
+      <xdr:colOff>2139120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>135360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6261480</xdr:colOff>
+      <xdr:colOff>6288120</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2396520</xdr:rowOff>
+      <xdr:rowOff>2387160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3967,8 +3967,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5223960" y="906120"/>
-          <a:ext cx="4149360" cy="2442600"/>
+          <a:off x="5250960" y="897120"/>
+          <a:ext cx="4149000" cy="2442240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3988,15 +3988,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>309600</xdr:colOff>
+      <xdr:colOff>336600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>111240</xdr:rowOff>
+      <xdr:rowOff>102240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>194400</xdr:colOff>
+      <xdr:colOff>221040</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4004,8 +4004,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="41981400" y="9248760"/>
-        <a:ext cx="5980680" cy="2884680"/>
+        <a:off x="42008400" y="9239760"/>
+        <a:ext cx="5980320" cy="2884320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4018,15 +4018,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>871560</xdr:colOff>
+      <xdr:colOff>898560</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2480040</xdr:colOff>
+      <xdr:colOff>2506680</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2402640</xdr:rowOff>
+      <xdr:rowOff>2393280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4039,8 +4039,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1074600" y="734760"/>
-          <a:ext cx="4517280" cy="2429640"/>
+          <a:off x="1101600" y="725760"/>
+          <a:ext cx="4516920" cy="2429280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4060,15 +4060,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>309600</xdr:colOff>
+      <xdr:colOff>336600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>111240</xdr:rowOff>
+      <xdr:rowOff>102240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>194400</xdr:colOff>
+      <xdr:colOff>221040</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4076,8 +4076,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="42260760" y="9163080"/>
-        <a:ext cx="5980680" cy="2884680"/>
+        <a:off x="42287760" y="9154080"/>
+        <a:ext cx="5980320" cy="2884320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4090,15 +4090,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>528840</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:colOff>555840</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1956600</xdr:colOff>
+      <xdr:colOff>1983240</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2318400</xdr:rowOff>
+      <xdr:rowOff>2309040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4111,8 +4111,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="731880" y="763200"/>
-          <a:ext cx="4336560" cy="2316960"/>
+          <a:off x="758880" y="754200"/>
+          <a:ext cx="4336200" cy="2316600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4132,15 +4132,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>163800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3375720</xdr:colOff>
+      <xdr:colOff>3402360</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1648440</xdr:rowOff>
+      <xdr:rowOff>1639080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4153,8 +4153,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81000" y="744120"/>
-          <a:ext cx="3294720" cy="1666080"/>
+          <a:off x="108000" y="735120"/>
+          <a:ext cx="3294360" cy="1665720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4169,15 +4169,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>804960</xdr:colOff>
+      <xdr:colOff>831960</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4394880</xdr:colOff>
+      <xdr:colOff>4421520</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1751760</xdr:rowOff>
+      <xdr:rowOff>1742400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4190,8 +4190,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5999760" y="734760"/>
-          <a:ext cx="3589920" cy="1778760"/>
+          <a:off x="6026760" y="725760"/>
+          <a:ext cx="3589560" cy="1778400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4211,15 +4211,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>432360</xdr:colOff>
+      <xdr:colOff>459000</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2187720</xdr:rowOff>
+      <xdr:rowOff>2178360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4232,8 +4232,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81000" y="906120"/>
-          <a:ext cx="4492080" cy="2214720"/>
+          <a:off x="108000" y="897120"/>
+          <a:ext cx="4491720" cy="2214360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4460,8 +4460,8 @@
   </sheetPr>
   <dimension ref="1:47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25065,7 +25065,7 @@
       </c>
       <c r="C21" s="29"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B22" s="30" t="s">
         <v>53</v>
       </c>
@@ -25077,7 +25077,7 @@
       <c r="AC22" s="0"/>
       <c r="AD22" s="0"/>
     </row>
-    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="32" t="s">
         <v>55</v>
       </c>
@@ -25089,7 +25089,7 @@
       <c r="AC23" s="0"/>
       <c r="AD23" s="0"/>
     </row>
-    <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="33" t="s">
         <v>57</v>
       </c>
@@ -25359,7 +25359,7 @@
   <dimension ref="B1:AD47"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25597,7 +25597,7 @@
       <c r="AC20" s="0"/>
       <c r="AD20" s="0"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B21" s="30" t="s">
         <v>53</v>
       </c>
@@ -25609,7 +25609,7 @@
       <c r="AC21" s="0"/>
       <c r="AD21" s="0"/>
     </row>
-    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="32" t="s">
         <v>55</v>
       </c>
@@ -25621,7 +25621,7 @@
       <c r="AC22" s="0"/>
       <c r="AD22" s="0"/>
     </row>
-    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="33" t="s">
         <v>57</v>
       </c>
@@ -28237,8 +28237,8 @@
   </sheetPr>
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>